<commit_message>
Falta probar el posible listener
</commit_message>
<xml_diff>
--- a/SpringBootFullStarter_2.3_PO/EspecificacionesPersistentObjects.xlsx
+++ b/SpringBootFullStarter_2.3_PO/EspecificacionesPersistentObjects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Java64\SpringBootFullStarter_2.3_PO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA49692-C729-478B-8752-A6F1C96277F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2A334F-62CD-4B42-9050-63026FC9BDF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{1600C9A1-0D5A-4CC6-A1A6-DCD13C90508D}"/>
+    <workbookView xWindow="1080" yWindow="2940" windowWidth="21600" windowHeight="11400" xr2:uid="{1600C9A1-0D5A-4CC6-A1A6-DCD13C90508D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -521,21 +521,22 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
@@ -549,7 +550,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -563,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -577,7 +578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -591,7 +592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -605,7 +606,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -619,7 +620,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -633,7 +634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -647,12 +648,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -666,7 +667,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -680,7 +681,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -694,7 +695,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>

</xml_diff>